<commit_message>
update phan chia cong viec
</commit_message>
<xml_diff>
--- a/GROUP 8 - Phân chia công việc .xlsx
+++ b/GROUP 8 - Phân chia công việc .xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e6b82f1ed0977918/Desktop/Group8_Capstone_Studious/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\long\Layout 5 - [CAPSTONE] LAYOUT BC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_B78E75BF745C1DFEC570D20FD4411CE2F5C887BC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CCB4283-9D83-462E-A955-3E8E2CAC34E2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -142,7 +141,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd"/>
   </numFmts>
@@ -301,23 +300,29 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,32 +537,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" customWidth="1"/>
-    <col min="8" max="8" width="6.44140625" customWidth="1"/>
-    <col min="9" max="9" width="16.5546875" customWidth="1"/>
-    <col min="10" max="10" width="25.6640625" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -588,271 +593,406 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="11">
-        <v>1</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="D2" s="10">
+        <v>1</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="12">
+        <v>44808</v>
+      </c>
+      <c r="G2" s="12">
+        <v>44808</v>
+      </c>
+      <c r="H2" s="10">
+        <v>1</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="13"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="11">
-        <v>1</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="D3" s="10">
+        <v>1</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="12">
+        <v>44808</v>
+      </c>
+      <c r="G3" s="12">
+        <v>44808</v>
+      </c>
+      <c r="H3" s="10">
+        <v>1</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="13"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="11">
-        <v>1</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="12">
+        <v>44808</v>
+      </c>
+      <c r="G4" s="12">
+        <v>44808</v>
+      </c>
+      <c r="H4" s="10">
+        <v>1</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="13"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="11">
-        <v>1</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="D5" s="10">
+        <v>1</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="12">
+        <v>44808</v>
+      </c>
+      <c r="G5" s="12">
+        <v>44808</v>
+      </c>
+      <c r="H5" s="10">
+        <v>1</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="13"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="B6" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="12">
+        <v>44808</v>
+      </c>
+      <c r="G6" s="12">
+        <v>44808</v>
+      </c>
+      <c r="H6" s="10">
+        <v>1</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="13"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="B7" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="10">
+        <v>1</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="12">
+        <v>44808</v>
+      </c>
+      <c r="G7" s="12">
+        <v>44808</v>
+      </c>
+      <c r="H7" s="10">
+        <v>1</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="13"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="13">
-        <v>1</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="D8" s="10">
+        <v>1</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="12">
         <v>44805</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="12">
         <v>44807</v>
       </c>
-      <c r="H8" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="H8" s="10">
+        <v>1</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="13"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="13">
-        <v>1</v>
-      </c>
-      <c r="E9" s="6" t="s">
+      <c r="D9" s="10">
+        <v>1</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="12">
         <v>44805</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="12">
         <v>44807</v>
       </c>
-      <c r="H9" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="H9" s="10">
+        <v>1</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="13"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="13">
-        <v>1</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="D10" s="10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="12">
         <v>44806</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="12">
         <v>44807</v>
       </c>
-      <c r="H10" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="H10" s="10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="13"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="13">
-        <v>1</v>
-      </c>
-      <c r="E11" s="6" t="s">
+      <c r="D11" s="10">
+        <v>1</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="12">
         <v>44806</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="12">
         <v>44807</v>
       </c>
-      <c r="H11" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="H11" s="10">
+        <v>1</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="13"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="13">
-        <v>1</v>
-      </c>
-      <c r="E12" s="6" t="s">
+      <c r="D12" s="10">
+        <v>1</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="12">
         <v>44807</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="12">
         <v>44807</v>
       </c>
-      <c r="H12" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="H12" s="10">
+        <v>1</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="13"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="6" t="s">
+      <c r="D13" s="10">
+        <v>1</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="12">
         <v>44807</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="12">
         <v>44807</v>
       </c>
-      <c r="H13" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="H13" s="10">
+        <v>1</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="12">
         <v>44807</v>
       </c>
-      <c r="C14" s="14">
-        <v>44808</v>
-      </c>
-      <c r="D14" s="13">
-        <v>1</v>
-      </c>
-      <c r="E14" s="6" t="s">
+      <c r="C14" s="12">
+        <v>44808</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="14">
-        <v>44808</v>
-      </c>
-      <c r="G14" s="14">
-        <v>44808</v>
-      </c>
-      <c r="H14" s="13">
-        <v>1</v>
-      </c>
+      <c r="F14" s="12">
+        <v>44808</v>
+      </c>
+      <c r="G14" s="12">
+        <v>44808</v>
+      </c>
+      <c r="H14" s="10">
+        <v>1</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>

</xml_diff>